<commit_message>
compare price v1, v3.0, v3.1, v3.3
</commit_message>
<xml_diff>
--- a/tests/datatest/listPools.xlsx
+++ b/tests/datatest/listPools.xlsx
@@ -8,20 +8,373 @@
   </bookViews>
   <sheets>
     <sheet name="Pools" sheetId="4" r:id="rId1"/>
-    <sheet name="Pools4" sheetId="1" r:id="rId2"/>
-    <sheet name="Pools (3)" sheetId="3" r:id="rId3"/>
-    <sheet name="Pools (2)" sheetId="2" r:id="rId4"/>
+    <sheet name="Pools (14)" sheetId="15" r:id="rId2"/>
+    <sheet name="Pools (13)" sheetId="14" r:id="rId3"/>
+    <sheet name="Pools (12)" sheetId="13" r:id="rId4"/>
+    <sheet name="Pools (11)" sheetId="12" r:id="rId5"/>
+    <sheet name="Pools (10)" sheetId="11" r:id="rId6"/>
+    <sheet name="Pools (9)" sheetId="10" r:id="rId7"/>
+    <sheet name="Pools (8)" sheetId="9" r:id="rId8"/>
+    <sheet name="Pools (7)" sheetId="8" r:id="rId9"/>
+    <sheet name="Pools (5)" sheetId="6" r:id="rId10"/>
+    <sheet name="Pools (6)" sheetId="7" r:id="rId11"/>
+    <sheet name="Pools (4)" sheetId="5" r:id="rId12"/>
+    <sheet name="Pools4" sheetId="1" r:id="rId13"/>
+    <sheet name="Pools (3)" sheetId="3" r:id="rId14"/>
+    <sheet name="Pools (2)" sheetId="2" r:id="rId15"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="225">
   <si>
     <t>list pools</t>
   </si>
   <si>
+    <t>{"messageType":"SplashG2Pool","result":{"pool":{"outRef":"ebee0c8d555f4e182a5f71bbdf7ab79e948c17d6508b49a333e38917c944b58d#0","address":"addr_test1xzw7upjedpkr4wq839wf983jsnq3yg40l4cskzd7dy8eyndj764lvrxdayh2ux30fl0ktuh27csgmpevdu89jlxppvrstmsqj2","coin":"5812812823","multiAssets":[{"policyId":"5cab70e3d5db96a649afb7184cdabd5df8395e29223308771e9ac292","assets":[{"name":"4144415f5553444d5f4c51","value":"9223372035931541773"}]},{"policyId":"baccbaa443f75f183d5ca59a37c1c5e19543183f5c6d8ae9efc6d036","assets":[{"name":"4144415f5553444d5f4e4654","value":"1"}]},{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"147840452"}]}],"refScriptOutRef":"482719d050a96b91206f78c6c2b834e844ea576557387e09e7b1c8afa4d433ac#0","validityNft":"baccbaa443f75f183d5ca59a37c1c5e19543183f5c6d8ae9efc6d036.4144415f5553444d5f4e4654","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","lpToken":"5cab70e3d5db96a649afb7184cdabd5df8395e29223308771e9ac292.4144415f5553444d5f4c51","poolFee":99730,"treasuryFee":30,"treasuryA":"2076512","treasuryB":"68886","daoPolicies":[],"treasuryAddressPkh":"75c4570eb625ae881b32a34c52b159f6f3f3f2c7aaabf5bac4688133"},"sequenceInfo":{"blockSlot":112943050,"transactionIndex":1},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:00:14.175</t>
+  </si>
+  <si>
+    <t>{"messageType":"SplashG3Pool","result":{"pool":{"outRef":"db9ecab0e20082ab421ddb4cba0b32e53449d7b80933566f5007defc83aff1d7#1","address":"addr_test1xz7n46v3kk40ejh7tjnswk9ax65m97rj74lk6wsllg8twaaj764lvrxdayh2ux30fl0ktuh27csgmpevdu89jlxppvrs04w48j","coin":"558829100261","multiAssets":[{"policyId":"82fdffb1016939f6d0c2a27b2393aafb6e310127c46fed48f664dc11","assets":[{"name":"665553444d5f4144415f4e4654","value":"1"}]},{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"148954786952"}]},{"policyId":"494926363f11ae6413e48ab65d8b3e6730e1e278991285547dbb391d","assets":[{"name":"665553444d5f4144415f4c51","value":"9223371753596942730"}]}],"refScriptOutRef":"2b7efe0f19eedbb94abb4e505d87fac41143b9422792aafdf5927c3535b303d4#1","validityNft":"82fdffb1016939f6d0c2a27b2393aafb6e310127c46fed48f664dc11.665553444d5f4144415f4e4654","tokenA":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","tokenB":"","lpToken":"494926363f11ae6413e48ab65d8b3e6730e1e278991285547dbb391d.665553444d5f4144415f4c51","poolFee":99100,"treasuryFee":50,"royaltyFee":50,"treasuryA":"165809411","treasuryB":"442250056","royaltyA":"165809411","royaltyB":"442250056","daoPolicies":[],"treasuryAddressPkh":"75c4570eb625ae881b32a34c52b159f6f3f3f2c7aaabf5bac4688133","royaltyAddressPkh":"72c68f905716a5f59a0ee2552ab68559f42287d335396d8f430da98e96c5009c","royaltyNonce":"0"},"sequenceInfo":{"blockSlot":113911186,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:00:14.178</t>
+  </si>
+  <si>
+    <t>{"messageType":"SplashG3Pool","result":{"pool":{"outRef":"b31023691c4bf82ccf53bcf1a7731979ed53fe1690559c0c52fa36e34993619b#0","address":"addr_test1xz7n46v3kk40ejh7tjnswk9ax65m97rj74lk6wsllg8twaaj764lvrxdayh2ux30fl0ktuh27csgmpevdu89jlxppvrs04w48j","coin":"6018183551","multiAssets":[{"policyId":"f5b262f983928c0dc5415fe1f90e4a20ffc5c2d5f3d21fcc5e021ebe","assets":[{"name":"4144415f5553444d5f4e46545f31","value":"1"}]},{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"1498362616"}]},{"policyId":"37ab398bfbdfe8a8d27f2dc7069475286f84df4f26183d70a0bacd42","assets":[{"name":"4144415f5553444d5f4c515f31","value":"9223372033980443278"}]}],"refScriptOutRef":"2b7efe0f19eedbb94abb4e505d87fac41143b9422792aafdf5927c3535b303d4#1","validityNft":"f5b262f983928c0dc5415fe1f90e4a20ffc5c2d5f3d21fcc5e021ebe.4144415f5553444d5f4e46545f31","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","lpToken":"37ab398bfbdfe8a8d27f2dc7069475286f84df4f26183d70a0bacd42.4144415f5553444d5f4c515f31","poolFee":91900,"treasuryFee":900,"royaltyFee":100,"treasuryA":"7570141","treasuryB":"955207","royaltyA":"841111","royaltyB":"106127","daoPolicies":[],"treasuryAddressPkh":"75c4570eb625ae881b32a34c52b159f6f3f3f2c7aaabf5bac4688133","royaltyAddressPkh":"72c68f905716a5f59a0ee2552ab68559f42287d335396d8f430da98e96c5009c","royaltyNonce":"0"},"sequenceInfo":{"blockSlot":112610339,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:00:14.186</t>
+  </si>
+  <si>
+    <t>{"messageType":"SplashG3Pool","result":{"pool":{"outRef":"dc3c6cbb319470b481ad65776619285268d96d02616d0c4f3d8863f714e2593d#3","address":"addr_test1xz7n46v3kk40ejh7tjnswk9ax65m97rj74lk6wsllg8twaaj764lvrxdayh2ux30fl0ktuh27csgmpevdu89jlxppvrs04w48j","coin":"5245194052","multiAssets":[{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"1327727217"}]},{"policyId":"77359874a76d9cb19d4ae24c60e5e4d71ecde489584c3d0ff68091fe","assets":[{"name":"4144415f5553444d5f4e46545f32","value":"1"}]},{"policyId":"2863e0da31ab4fb792394b6ef9997c9235bdb7a64102dde9dd33d690","assets":[{"name":"4144415f5553444d5f4c515f32","value":"9223372033980443278"}]}],"refScriptOutRef":"2b7efe0f19eedbb94abb4e505d87fac41143b9422792aafdf5927c3535b303d4#1","validityNft":"77359874a76d9cb19d4ae24c60e5e4d71ecde489584c3d0ff68091fe.4144415f5553444d5f4e46545f32","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","lpToken":"2863e0da31ab4fb792394b6ef9997c9235bdb7a64102dde9dd33d690.4144415f5553444d5f4c515f32","poolFee":91900,"treasuryFee":900,"royaltyFee":100,"treasuryA":"4707400","treasuryB":"1249221","royaltyA":"523038","royaltyB":"138797","daoPolicies":[],"treasuryAddressPkh":"75c4570eb625ae881b32a34c52b159f6f3f3f2c7aaabf5bac4688133","royaltyAddressPkh":"72c68f905716a5f59a0ee2552ab68559f42287d335396d8f430da98e96c5009c","royaltyNonce":"0"},"sequenceInfo":{"blockSlot":112590329,"transactionIndex":2},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:00:14.189</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"6af7e207a738b1637132c4d0216918a8b91408f571d3f2870d0f5a9ee324e063#1","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vy2v94fpsddtn0xtkq4vj04sergmm5pz5pzcz6y82pvkzgqn89mn9","coin":"164714548","multiAssets":[{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"9a2e6155e399fd7f9e1810195b55f5730ff9b7b7280a094accb5e48ce0f2926a","value":"1"}]},{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"6024438"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.9a2e6155e399fd7f9e1810195b55f5730ff9b7b7280a094accb5e48ce0f2926a","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"23923183896578434","sqrtPriceLowerDen":"100000000000000000","sqrtPriceUpperNum":"32601804202361095","sqrtPriceUpperDen":"100000000000000000","poolFeeRate":10,"platformFeeRate":500,"platformFeeA":"24945","platformFeeB":"7690","minTxAmountA":"38662483","minTxAmountB":"3161037","circulatingLpToken":"97000000","lastWithdrawEpoch":67933,"stakingUtxo":{"outRef":"1178ae4595526868d0c0ed98d8aa470980370b9f4aa1be7c340b7fb67e8a5fb8#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113906468,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:00:14.191</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"6af7e207a738b1637132c4d0216918a8b91408f571d3f2870d0f5a9ee324e063#0","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vqdax6vmwwwj6wcj2yzqpjs7thun50vxynuh0vpfy3zzegqsjka7n","coin":"44691699","multiAssets":[{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"3956022"}]},{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"3126f6b928ae5aa7dc25d82d98a6fd8ed8fdce26885481e84f7bd358583d93af","value":"1"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.3126f6b928ae5aa7dc25d82d98a6fd8ed8fdce26885481e84f7bd358583d93af","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"21520116174491596","sqrtPriceLowerDen":"100000000000000000","sqrtPriceUpperNum":"29326974911277726","sqrtPriceUpperDen":"100000000000000000","poolFeeRate":10,"platformFeeRate":500,"platformFeeA":"4500","platformFeeB":"300","minTxAmountA":"42979773","minTxAmountB":"2843513","circulatingLpToken":"41795764","lastWithdrawEpoch":67933,"stakingUtxo":{"outRef":"b450aacb59445d0081d994f828608769053fc0f8aa4bcdaa889803719bebd049#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113906468,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:00:14.196</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"6af7e207a738b1637132c4d0216918a8b91408f571d3f2870d0f5a9ee324e063#7","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vpd4pl6sta79ykcgxx065c3lycgwy9xm34vajm5x8vw6ldsde3rrc","coin":"1006038108","multiAssets":[{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"147653302883"}]},{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"c4d966b065db0887d643f2992e82f8dc4782d0829ffaa3856998824037e710f9","value":"1"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.c4d966b065db0887d643f2992e82f8dc4782d0829ffaa3856998824037e710f9","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"24374579270728639","sqrtPriceLowerDen":"100000000000000000","sqrtPriceUpperNum":"33216952406275596","sqrtPriceUpperDen":"100000000000000000","poolFeeRate":10,"platformFeeRate":500,"platformFeeA":"987216","platformFeeB":"185185","minTxAmountA":"37946489","minTxAmountB":"3220681","circulatingLpToken":"701214764746","lastWithdrawEpoch":67933,"stakingUtxo":{"outRef":"02d4e9025876902fc2ee6c6b8e13f6a3ef444c8b6a89f8805833bb956415f832#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113906468,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:00:14.197</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"6af7e207a738b1637132c4d0216918a8b91408f571d3f2870d0f5a9ee324e063#6","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vyuxcade0jfkhtz7e6mzqzw6c3a9r6h9mht3jt7mhe70sqq703vum","coin":"14431497210","multiAssets":[{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"1113376674"}]},{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"15924768fc822a4b15df3b487738c41934f544dfc8aa6bfe692e2da39f7c4511","value":"1"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.15924768fc822a4b15df3b487738c41934f544dfc8aa6bfe692e2da39f7c4511","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"17320508075688773","sqrtPriceLowerDen":"100000000000000000","sqrtPriceUpperNum":"9486832980505138","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":10,"platformFeeRate":500,"platformFeeA":"1377669","platformFeeB":"391616","minTxAmountA":"39501417","minTxAmountB":"3093903","circulatingLpToken":"18101093419","lastWithdrawEpoch":67933,"stakingUtxo":{"outRef":"f7bf1318abd11ff715abda8fedf164690241941f4dcce6d963b6ac59dc862cfc#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113906468,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:00:14.200</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"6af7e207a738b1637132c4d0216918a8b91408f571d3f2870d0f5a9ee324e063#5","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vprnxs9yt369fqkyjq79t0qyzp5hrzn04cqlet4vhdsluzqwkehk0","coin":"3560274609","multiAssets":[{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"396587349"}]},{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"470437a5df9d8d3c4dc110d2f4f4d80d0082e6f68f91103fbc5412943423769e","value":"1"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.470437a5df9d8d3c4dc110d2f4f4d80d0082e6f68f91103fbc5412943423769e","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"1000000","sqrtPriceLowerDen":"10000000","sqrtPriceUpperNum":"9486832980505138","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":30,"platformFeeRate":500,"platformFeeA":"722865","platformFeeB":"147836","minTxAmountA":"37946489","minTxAmountB":"3220681","circulatingLpToken":"4068927185","lastWithdrawEpoch":67933,"stakingUtxo":{"outRef":"3f8a54141bfc7b46a245b8c487e9259433c198067de8ff16843cd67f0bfdd77a#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113906468,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:00:14.202</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"6af7e207a738b1637132c4d0216918a8b91408f571d3f2870d0f5a9ee324e063#4","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vx25zajjegptl98gtd6xs6uduuf5qqmtz6ekp0n8sltjc7q3gmyyy","coin":"56967560","multiAssets":[{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"56154116"}]},{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"d0c20b099ebdb52aba221386deda5f4930f9b72aa1221ccd2d0973a70d02badc","value":"1"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.d0c20b099ebdb52aba221386deda5f4930f9b72aa1221ccd2d0973a70d02badc","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"20677736735999433","sqrtPriceLowerDen":"100000000000000000","sqrtPriceUpperNum":"2817900524149877","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":10,"platformFeeRate":500,"platformFeeA":"98071","platformFeeB":"7715","minTxAmountA":"44730703","minTxAmountB":"2732207","circulatingLpToken":"397000000","lastWithdrawEpoch":67933,"stakingUtxo":{"outRef":"cfec8ec1e6c424afd9b724ba58552c5f781e83fc6df3fa73996c5960dd88c321#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113906468,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:00:14.204</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"6af7e207a738b1637132c4d0216918a8b91408f571d3f2870d0f5a9ee324e063#3","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04v8yrwvdzwuumq0lcgphg2v357jnrwq876nezlt4349jcneq23lzrm","coin":"56870935","multiAssets":[{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"53136824"}]},{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"e57a5327ebc6c80248dd4fac8ce4c4bb318daf7bc2195a9ad59a21eccfe123d0","value":"1"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.e57a5327ebc6c80248dd4fac8ce4c4bb318daf7bc2195a9ad59a21eccfe123d0","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"20677736735999433","sqrtPriceLowerDen":"100000000000000000","sqrtPriceUpperNum":"2817900524149877","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":10,"platformFeeRate":500,"platformFeeA":"94018","platformFeeB":"7410","minTxAmountA":"44730703","minTxAmountB":"2732207","circulatingLpToken":"376108224","lastWithdrawEpoch":67933,"stakingUtxo":{"outRef":"62c21ad53ba10d49b57e2733cfc2f8f2461c743a3de3bd1bff5e6d9fd37ace3e#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113906468,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:00:14.205</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"6af7e207a738b1637132c4d0216918a8b91408f571d3f2870d0f5a9ee324e063#2","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vyunnxqnevxe0ufjaxmwyakld723canz56wg2prqh2n27us3506ft","coin":"51622433","multiAssets":[{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"11341112"}]},{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"26f11dbf94cf846cb34cc0572b857ffc626adf61c42d0b60a549d67f09431758","value":"1"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.26f11dbf94cf846cb34cc0572b857ffc626adf61c42d0b60a549d67f09431758","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"20677736735999433","sqrtPriceLowerDen":"100000000000000000","sqrtPriceUpperNum":"2817900524149877","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":10,"platformFeeRate":500,"platformFeeA":"38699","platformFeeB":"3142","minTxAmountA":"44730703","minTxAmountB":"2732207","circulatingLpToken":"97000000","lastWithdrawEpoch":67933,"stakingUtxo":{"outRef":"f9c82a78645d57d4afcdec482fe5b9fc2565da53e511614109484b2836c14cbe#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113906468,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:00:14.207</t>
+  </si>
+  <si>
+    <t>{"messageType":"FloatProtocolConfig","result":{"protocolConfig":{"protocolConfigOutRef":"633ff0cb3ad4ca197e457ba051265b9aa6f6fb45d240556741ae551fda4693ea#0","poolScriptHash":"6b3b8633c908d7dc170155da323d0008bfb76d5e123192360830ca8d","poolScriptOutRef":"d9cf6b2d222eaf86afd97de6e0f150ec252031a8c6dbac9253d99f45d883a837#0","loanScriptHash":"6d581cda24be77402905f206a163395a2cec8308098f4e9b290ef57a","loanScriptOutRef":"d8dc1fcc5fcec28d043b7658797b081c85bdbd42140839d5bab0c58cb7b000f6#0","poolParamScriptHash":"e5e9120138ff062befc0b55f840dc632e4ccac51740600d78403273a","poolParamScriptOutRef":"cfd265e482273df1702acf126c3d97d96933a347d101acbef144a956e03abee4#0","oraclePriceScriptHash":"0fb1126ccc889bc4c338e84e1e3485e3f207e532cb2c7861899efdd0","oraclePriceScriptOutRef":"a084460ca6042f1c3f35feba76895300f4bb3278ff3fd09c2e952485c6ac7b8c#0","loanOwnerNftMetadata":{"name":"Borrower NFT (Flexible Pool Lending)","image":"ipfs://bafkreicqj5oanntibwf3wupgejc2nxiphyvaz5gk3jpsaolebnawhyuoea","description":"An NFT representing the loan from the Danogo Flexible Pool Lending"}},"sequenceInfo":{"blockSlot":0,"transactionIndex":0},"isSpent":null}}</t>
+  </si>
+  <si>
+    <t>17:00:14.210</t>
+  </si>
+  <si>
+    <t>{"messageType":"FloatPool","result":{"pool":{"outRef":"db9ecab0e20082ab421ddb4cba0b32e53449d7b80933566f5007defc83aff1d7#2","address":"addr_test1wp4nhp3neyyd0hqhq92a5v3aqqytldmdtcfrry3kpqcv4rgt8arjt","coin":"5000001","multiAssets":[{"policyId":"703d581d9a657d1326aea6a754cdcf191efb22133a62a181951156cf","assets":[{"name":"","value":"32246074819"}]},{"policyId":"e5e9120138ff062befc0b55f840dc632e4ccac51740600d78403273a","assets":[{"name":"435a1f498bf490359a86e94918cb09806d9c28d85d0b44659061ff4a","value":"1"}]}],"poolId":"e5e9120138ff062befc0b55f840dc632e4ccac51740600d78403273a.435a1f498bf490359a86e94918cb09806d9c28d85d0b44659061ff4a","dToken":"6b3b8633c908d7dc170155da323d0008bfb76d5e123192360830ca8d.435a1f498bf490359a86e94918cb09806d9c28d85d0b44659061ff4a","totalSupply":"277128333100","circulatingDToken":"262627842695","totalBorrow":"244224909588","borrowApy":1178,"undistributedFee":"0","interestIndex":"1195529023420","interestTime":"1769594218000","alternativeSupplyTokens":[{"latestExchangeRateNum":"43555813947","latestExchangeRateDen":"42685649457"}]},"marketToken":"","sequenceInfo":{"blockSlot":113911186,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:00:14.213</t>
+  </si>
+  <si>
+    <t>{"messageType":"FloatPool","result":{"pool":{"outRef":"4be5193730cfb9e3229fc00109c3989f84f33d8171cbdf58c5a82beab15fa2b9#1","address":"addr_test1wp4nhp3neyyd0hqhq92a5v3aqqytldmdtcfrry3kpqcv4rgt8arjt","coin":"5000000","multiAssets":[{"policyId":"e5e9120138ff062befc0b55f840dc632e4ccac51740600d78403273a","assets":[{"name":"520aa368b4b171ee9de426e3e1ff568b1f5cf77d77f97ef7066bcb59","value":"1"}]}],"poolId":"e5e9120138ff062befc0b55f840dc632e4ccac51740600d78403273a.520aa368b4b171ee9de426e3e1ff568b1f5cf77d77f97ef7066bcb59","dToken":"6b3b8633c908d7dc170155da323d0008bfb76d5e123192360830ca8d.520aa368b4b171ee9de426e3e1ff568b1f5cf77d77f97ef7066bcb59","totalSupply":"0","circulatingDToken":"0","totalBorrow":"0","borrowApy":100,"undistributedFee":"0","interestIndex":"1000000000000","interestTime":"1758705510000","alternativeSupplyTokens":[]},"marketToken":"","sequenceInfo":{"blockSlot":103022402,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:00:14.215</t>
+  </si>
+  <si>
+    <t>{"messageType":"FloatPoolParam","result":{"poolParam":{"outRef":"6f6ba786233d819ae768f8f2a1f9eb0b121f6d8eebe87e0c3ff8a459c0fc67e4#0","address":"addr_test1wrj7jysp8rlsv2l0cz64lpqdccewfn9v296qvqxhsspjwwslx7k0s","coin":"5434910","multiAssets":[{"policyId":"e5e9120138ff062befc0b55f840dc632e4ccac51740600d78403273a","assets":[{"name":"435a1f498bf490359a86e94918cb09806d9c28d85d0b44659061ff4a","value":"1"}]}],"poolId":"e5e9120138ff062befc0b55f840dc632e4ccac51740600d78403273a.435a1f498bf490359a86e94918cb09806d9c28d85d0b44659061ff4a","baseInterestRate":300,"powerBase":10250,"minTxAmount":"99999995","utilizationCap":9000,"loanFeeRate":1000,"loanOriginationFeeRate":10,"withdrawalFee":"0","loanOriginationFeeMinAmount":"5000000","feeAddress":"addr_test1qr20zc2v0fyxwjf42jy8vjctfpqrc9f3md3cwe6fccsza9g5q42ut28rqch23fj0j4hp479jdkeyn2mpv8tmxk3h5jeqsm9xmy","liquidatorRewardCap":100,"collectorReward":"4000000","supportedCollaterals":[{"token":"d2a8592ec9673ac18fea1044885f94518e954ab0cb2b6bb0a328d2af.425443","liquidationThreshold":9250,"minSupplyAmount":"0","isEnable":true},{"token":"e16c2dc8ae937e8d3790c7fd7168d7b994621ba14ca11415f39fed72.4d494e","liquidationThreshold":9250,"minSupplyAmount":"0","isEnable":false},{"token":"9de4aa80ab5b2223cc6f31652204c9451f9db7d3336db5681316f9f5.66455448","liquidationThreshold":9250,"minSupplyAmount":"0","isEnable":true},{"token":"007c4fc75b7662fc735177aa714da9d1b06af5644df199fef39e5fc1.66425443","liquidationThreshold":9250,"minSupplyAmount":"0","isEnable":true},{"token":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","liquidationThreshold":9250,"minSupplyAmount":"0","isEnable":true},{"token":"9a614be30284aa88eb845da7657b5d0a235f1b95628b23c08050d502.6655534441","liquidationThreshold":9250,"minSupplyAmount":"0","isEnable":true},{"token":"6b3b8633c908d7dc170155da323d0008bfb76d5e123192360830ca8d.d08f0e1ce65885dcadd082b87e5f6e26927263c9b6cd4c56384e894f","liquidationThreshold":8000,"minSupplyAmount":"0","isEnable":false},{"token":"6b3b8633c908d7dc170155da323d0008bfb76d5e123192360830ca8d.db56b4792136b01b45a54d38576e094c9d0d06586969daf6a4979ce1","liquidationThreshold":8000,"minSupplyAmount":"0","isEnable":true},{"token":"6b3b8633c908d7dc170155da323d0008bfb76d5e123192360830ca8d.fa21c4c67475fa0729a80d176634c4673e94867818ae76d8a6326aca","liquidationThreshold":8000,"minSupplyAmount":"0","isEnable":true},{"token":"6b3b8633c908d7dc170155da323d0008bfb76d5e123192360830ca8d.435a1f498bf490359a86e94918cb09806d9c28d85d0b44659061ff4a","liquidationThreshold":8000,"minSupplyAmount":"0","isEnable":true},{"token":"6b3b8633c908d7dc170155da323d0008bfb76d5e123192360830ca8d.44aa97ebe2d8d22955423890f2dc4fc125e3cc5c70dd8c1c01b73a02","liquidationThreshold":8000,"minSupplyAmount":"0","isEnable":true},{"token":"6b3b8633c908d7dc170155da323d0008bfb76d5e123192360830ca8d.4671f6fe1ce54e960c62840747872b0e2892061f00942afe646008e3","liquidationThreshold":8000,"minSupplyAmount":"0","isEnable":true},{"token":"6b3b8633c908d7dc170155da323d0008bfb76d5e123192360830ca8d.59f3a03847e9c1646a2a55609fdcee8ba9a69065e8f9aaf1a16b0f86","liquidationThreshold":8000,"minSupplyAmount":"0","isEnable":true},{"token":"6b3b8633c908d7dc170155da323d0008bfb76d5e123192360830ca8d.6667926a8b819f3c96652574103f59c9847b85d56e78f10933cad3bc","liquidationThreshold":8000,"minSupplyAmount":"0","isEnable":false}],"alternativeSupplyTokens":[{"token":"703d581d9a657d1326aea6a754cdcf191efb22133a62a181951156cf","isEnable":true}]},"marketToken":"","sequenceInfo":{"blockSlot":111637501,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:00:14.217</t>
+  </si>
+  <si>
+    <t>{"method":"subscribeOracleEvent","params":{"type":"nioblockchain.tradingaggregator.model.OracleEvent","tokenPairs":[{"baseToken":"703d581d9a657d1326aea6a754cdcf191efb22133a62a181951156cf","quoteToken":""}]}}</t>
+  </si>
+  <si>
+    <t>17:00:14.223</t>
+  </si>
+  <si>
+    <t>{"messageType":"FloatPoolParam","result":{"poolParam":{"outRef":"befd26008b6a967a9ad480611100c5e01bd82ef0437648cd563c76e6f5db2273#0","address":"addr_test1wrj7jysp8rlsv2l0cz64lpqdccewfn9v296qvqxhsspjwwslx7k0s","coin":"2086040","multiAssets":[{"policyId":"e5e9120138ff062befc0b55f840dc632e4ccac51740600d78403273a","assets":[{"name":"520aa368b4b171ee9de426e3e1ff568b1f5cf77d77f97ef7066bcb59","value":"1"}]}],"poolId":"e5e9120138ff062befc0b55f840dc632e4ccac51740600d78403273a.520aa368b4b171ee9de426e3e1ff568b1f5cf77d77f97ef7066bcb59","baseInterestRate":100,"powerBase":10200,"minTxAmount":"99","utilizationCap":9000,"loanFeeRate":1000,"loanOriginationFeeRate":0,"withdrawalFee":"0","loanOriginationFeeMinAmount":"0","feeAddress":"addr_test1qr20zc2v0fyxwjf42jy8vjctfpqrc9f3md3cwe6fccsza9g5q42ut28rqch23fj0j4hp479jdkeyn2mpv8tmxk3h5jeqsm9xmy","liquidatorRewardCap":1000,"collectorReward":"0","supportedCollaterals":[{"token":"","liquidationThreshold":8000,"minSupplyAmount":"0","isEnable":true},{"token":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","liquidationThreshold":8000,"minSupplyAmount":"0","isEnable":true},{"token":"9a614be30284aa88eb845da7657b5d0a235f1b95628b23c08050d502.6655534441","liquidationThreshold":6000,"minSupplyAmount":"0","isEnable":true}],"alternativeSupplyTokens":[]},"marketToken":"","sequenceInfo":{"blockSlot":103184845,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:00:14.224</t>
+  </si>
+  <si>
+    <t>{"method":"subscribeOracleEvent","params":{"type":"nioblockchain.tradingaggregator.model.OracleEvent","tokenPairs":[{"baseToken":"","quoteToken":""}]}}</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"cba60afd6a7ec9715f5d9f7d2632827ea774fe1a88790de2615b025f1f4b269d#0","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04v9t5afd2p9kwwc5yxf43lxctvcc7gy85h3std0ytua7ryjsgd5t3y","coin":"8201761845","multiAssets":[{"policyId":"9a614be30284aa88eb845da7657b5d0a235f1b95628b23c08050d502","assets":[{"name":"6655534441","value":"8644383029"}]},{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"552900ed12d0d2ece162ae5bf7232e22e18773d230e74aab2c33b654db22995b","value":"1"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.552900ed12d0d2ece162ae5bf7232e22e18773d230e74aab2c33b654db22995b","tokenA":"","tokenB":"9a614be30284aa88eb845da7657b5d0a235f1b95628b23c08050d502.6655534441","sqrtPriceLowerNum":"4424174411190986","sqrtPriceLowerDen":"10000000000000000","sqrtPriceUpperNum":"6029133435344022","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":50,"platformFeeRate":500,"platformFeeA":"2342593","platformFeeB":"714399","minTxAmountA":"39012600","minTxAmountB":"10908658","circulatingLpToken":"16386560851","lastWithdrawEpoch":67875,"stakingUtxo":{"outRef":"800b132bfefbeb309328d2db514beb01bb2c6f1cdad4f0b26d1f3d43c35dc810#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113800982,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>11:49:58.848</t>
+  </si>
+  <si>
+    <t>swap 40</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"949a1176aaa7eab2f31df17ccf01a8ba7b56cf7383d7022a7c6ad4b2e36703fd#0","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vyk5dchccgw9hcsmcwyvrgnf6jx3nuncvfxc6525u0ad2jsxfkpn7","coin":"12950972753","multiAssets":[{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"7c90426e2f22f721c79fa481e671c88cdddf6af4d6fbac734f95cf0cca9f3a96","value":"1"}]},{"policyId":"9a614be30284aa88eb845da7657b5d0a235f1b95628b23c08050d502","assets":[{"name":"6655534441","value":"13634078"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.7c90426e2f22f721c79fa481e671c88cdddf6af4d6fbac734f95cf0cca9f3a96","tokenA":"","tokenB":"9a614be30284aa88eb845da7657b5d0a235f1b95628b23c08050d502.6655534441","sqrtPriceLowerNum":"1670317415786537","sqrtPriceLowerDen":"1000000000000000","sqrtPriceUpperNum":"22762589453260365","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":100,"platformFeeRate":500,"platformFeeA":"378452","platformFeeB":"180855","minTxAmountA":"43478202","minTxAmountB":"10908665","circulatingLpToken":"34688135297","lastWithdrawEpoch":67829,"stakingUtxo":{"outRef":"18bf8a7d5fcd47daea94341df1f4d38b674c6ad5f0bcf12ee5289a58d73cf527#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113718022,"transactionIndex":1},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>11:49:58.850</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"6613968736852bec8511386427b31857c74aa2989fdc42e09e338c4c92808919#0","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vxprf078zm0k3jagzlnxf0emduy4k6da8pmd347t63xuywsr3s5fs","coin":"33096693610","multiAssets":[{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"6c02c67d3deddd62c868cebedece6f71df268c51013203c1140a4cd97261185c","value":"1"}]},{"policyId":"9a614be30284aa88eb845da7657b5d0a235f1b95628b23c08050d502","assets":[{"name":"6655534441","value":"4241282232"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.6c02c67d3deddd62c868cebedece6f71df268c51013203c1140a4cd97261185c","tokenA":"","tokenB":"9a614be30284aa88eb845da7657b5d0a235f1b95628b23c08050d502.6655534441","sqrtPriceLowerNum":"5251030279859372","sqrtPriceLowerDen":"10000000000000000","sqrtPriceUpperNum":"6808116479614608","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":30,"platformFeeRate":500,"platformFeeA":"2200376","platformFeeB":"685355","minTxAmountA":"39012600","minTxAmountB":"10908658","circulatingLpToken":"45371802092","lastWithdrawEpoch":67877,"stakingUtxo":{"outRef":"da4884bf928284f5860c784c8abdecbfb3707f70763438d5f7400432782d6ff4#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113805707,"transactionIndex":1},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>10:40:40.219</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"2beee63dc3d1b3000c4411cba69707d4fe0a5f98ba9244dcc42acbc81886a5b0#0","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vxprf078zm0k3jagzlnxf0emduy4k6da8pmd347t63xuywsr3s5fs","coin":"33253500520","multiAssets":[{"policyId":"9a614be30284aa88eb845da7657b5d0a235f1b95628b23c08050d502","assets":[{"name":"6655534441","value":"4191282232"}]},{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"6c02c67d3deddd62c868cebedece6f71df268c51013203c1140a4cd97261185c","value":"1"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.6c02c67d3deddd62c868cebedece6f71df268c51013203c1140a4cd97261185c","tokenA":"","tokenB":"9a614be30284aa88eb845da7657b5d0a235f1b95628b23c08050d502.6655534441","sqrtPriceLowerNum":"5251030279859372","sqrtPriceLowerDen":"10000000000000000","sqrtPriceUpperNum":"6808116479614608","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":30,"platformFeeRate":500,"platformFeeA":"2200376","platformFeeB":"677855","minTxAmountA":"39012600","minTxAmountB":"10908658","circulatingLpToken":"45371802092","lastWithdrawEpoch":67875,"stakingUtxo":{"outRef":"da4884bf928284f5860c784c8abdecbfb3707f70763438d5f7400432782d6ff4#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113802100,"transactionIndex":2},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>11:40:09.843</t>
+  </si>
+  <si>
+    <t>11:40:09.845</t>
+  </si>
+  <si>
+    <t>{"messageType":"SplashG3Pool","result":{"pool":{"outRef":"ddfb7a84c1358eb0d1ef71ab0415879bc95b26274e6ef63e812581ac320acba3#2","address":"addr_test1xz7n46v3kk40ejh7tjnswk9ax65m97rj74lk6wsllg8twaaj764lvrxdayh2ux30fl0ktuh27csgmpevdu89jlxppvrs04w48j","coin":"299817632899","multiAssets":[{"policyId":"97a4d074cf79ad8c55937b78af393b4caa2de06ce248df4aaef155f3","assets":[{"name":"66555344415f4144415f4c51","value":"9223371753596942730"}]},{"policyId":"a130d090656bb79c2671f004a6fe2b69f5f03cc28e61528b06b190c8","assets":[{"name":"66555344415f4144415f4e4654","value":"1"}]},{"policyId":"9a614be30284aa88eb845da7657b5d0a235f1b95628b23c08050d502","assets":[{"name":"6655534441","value":"267614322787"}]}],"refScriptOutRef":"2b7efe0f19eedbb94abb4e505d87fac41143b9422792aafdf5927c3535b303d4#1","validityNft":"a130d090656bb79c2671f004a6fe2b69f5f03cc28e61528b06b190c8.66555344415f4144415f4e4654","tokenA":"9a614be30284aa88eb845da7657b5d0a235f1b95628b23c08050d502.6655534441","tokenB":"","lpToken":"97a4d074cf79ad8c55937b78af393b4caa2de06ce248df4aaef155f3.66555344415f4144415f4c51","poolFee":99100,"treasuryFee":50,"royaltyFee":50,"treasuryA":"82156","treasuryB":"0","royaltyA":"82156","royaltyB":"0","daoPolicies":[],"treasuryAddressPkh":"75c4570eb625ae881b32a34c52b159f6f3f3f2c7aaabf5bac4688133","royaltyAddressPkh":"72c68f905716a5f59a0ee2552ab68559f42287d335396d8f430da98e96c5009c","royaltyNonce":"0"},"sequenceInfo":{"blockSlot":106039872,"transactionIndex":3},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>10:40:40.209</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"2e50c0bafe40ef893389bd3bb571b6630748e506ce2e41c63f13118367ef935d#0","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vxprf078zm0k3jagzlnxf0emduy4k6da8pmd347t63xuywsr3s5fs","coin":"33185500522","multiAssets":[{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"6c02c67d3deddd62c868cebedece6f71df268c51013203c1140a4cd97261185c","value":"1"}]},{"policyId":"9a614be30284aa88eb845da7657b5d0a235f1b95628b23c08050d502","assets":[{"name":"6655534441","value":"4212825123"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.6c02c67d3deddd62c868cebedece6f71df268c51013203c1140a4cd97261185c","tokenA":"","tokenB":"9a614be30284aa88eb845da7657b5d0a235f1b95628b23c08050d502.6655534441","sqrtPriceLowerNum":"5251030279859372","sqrtPriceLowerDen":"10000000000000000","sqrtPriceUpperNum":"6808116479614608","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":30,"platformFeeRate":500,"platformFeeA":"2190177","platformFeeB":"677855","minTxAmountA":"39012600","minTxAmountB":"10908658","circulatingLpToken":"45371802092","lastWithdrawEpoch":67875,"stakingUtxo":{"outRef":"da4884bf928284f5860c784c8abdecbfb3707f70763438d5f7400432782d6ff4#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113800881,"transactionIndex":1},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>10:40:40.216</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"949a1176aaa7eab2f31df17ccf01a8ba7b56cf7383d7022a7c6ad4b2e36703fd#0","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vyk5dchccgw9hcsmcwyvrgnf6jx3nuncvfxc6525u0ad2jsxfkpn7","coin":"12950972753","multiAssets":[{"policyId":"9a614be30284aa88eb845da7657b5d0a235f1b95628b23c08050d502","assets":[{"name":"6655534441","value":"13634078"}]},{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"7c90426e2f22f721c79fa481e671c88cdddf6af4d6fbac734f95cf0cca9f3a96","value":"1"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.7c90426e2f22f721c79fa481e671c88cdddf6af4d6fbac734f95cf0cca9f3a96","tokenA":"","tokenB":"9a614be30284aa88eb845da7657b5d0a235f1b95628b23c08050d502.6655534441","sqrtPriceLowerNum":"1670317415786537","sqrtPriceLowerDen":"1000000000000000","sqrtPriceUpperNum":"22762589453260365","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":100,"platformFeeRate":500,"platformFeeA":"378452","platformFeeB":"180855","minTxAmountA":"43478202","minTxAmountB":"10908665","circulatingLpToken":"34688135297","lastWithdrawEpoch":67829,"stakingUtxo":{"outRef":"18bf8a7d5fcd47daea94341df1f4d38b674c6ad5f0bcf12ee5289a58d73cf527#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113718022,"transactionIndex":1},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>10:40:40.218</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"cba60afd6a7ec9715f5d9f7d2632827ea774fe1a88790de2615b025f1f4b269d#0","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04v9t5afd2p9kwwc5yxf43lxctvcc7gy85h3std0ytua7ryjsgd5t3y","coin":"8201761845","multiAssets":[{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"552900ed12d0d2ece162ae5bf7232e22e18773d230e74aab2c33b654db22995b","value":"1"}]},{"policyId":"9a614be30284aa88eb845da7657b5d0a235f1b95628b23c08050d502","assets":[{"name":"6655534441","value":"8644383029"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.552900ed12d0d2ece162ae5bf7232e22e18773d230e74aab2c33b654db22995b","tokenA":"","tokenB":"9a614be30284aa88eb845da7657b5d0a235f1b95628b23c08050d502.6655534441","sqrtPriceLowerNum":"4424174411190986","sqrtPriceLowerDen":"10000000000000000","sqrtPriceUpperNum":"6029133435344022","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":50,"platformFeeRate":500,"platformFeeA":"2342593","platformFeeB":"714399","minTxAmountA":"39012600","minTxAmountB":"10908658","circulatingLpToken":"16386560851","lastWithdrawEpoch":67875,"stakingUtxo":{"outRef":"800b132bfefbeb309328d2db514beb01bb2c6f1cdad4f0b26d1f3d43c35dc810#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113800982,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>{"messageType":"SplashG3Pool","result":{"pool":{"outRef":"4946dc95ead86af1c7778fe087ea944bdef7943fecb1fc94005c33bfa8b5b65d#1","address":"addr_test1xz7n46v3kk40ejh7tjnswk9ax65m97rj74lk6wsllg8twaaj764lvrxdayh2ux30fl0ktuh27csgmpevdu89jlxppvrs04w48j","coin":"555809948914","multiAssets":[{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"149733755636"}]},{"policyId":"494926363f11ae6413e48ab65d8b3e6730e1e278991285547dbb391d","assets":[{"name":"665553444d5f4144415f4c51","value":"9223371753596942730"}]},{"policyId":"82fdffb1016939f6d0c2a27b2393aafb6e310127c46fed48f664dc11","assets":[{"name":"665553444d5f4144415f4e4654","value":"1"}]}],"refScriptOutRef":"2b7efe0f19eedbb94abb4e505d87fac41143b9422792aafdf5927c3535b303d4#1","validityNft":"82fdffb1016939f6d0c2a27b2393aafb6e310127c46fed48f664dc11.665553444d5f4144415f4e4654","tokenA":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","tokenB":"","lpToken":"494926363f11ae6413e48ab65d8b3e6730e1e278991285547dbb391d.665553444d5f4144415f4c51","poolFee":99100,"treasuryFee":50,"royaltyFee":50,"treasuryA":"165270993","treasuryB":"438724836","royaltyA":"165270993","royaltyB":"438724836","daoPolicies":[],"treasuryAddressPkh":"75c4570eb625ae881b32a34c52b159f6f3f3f2c7aaabf5bac4688133","royaltyAddressPkh":"72c68f905716a5f59a0ee2552ab68559f42287d335396d8f430da98e96c5009c","royaltyNonce":"0"},"sequenceInfo":{"blockSlot":113736584,"transactionIndex":1},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:46:25.255</t>
+  </si>
+  <si>
+    <t>17:46:25.260</t>
+  </si>
+  <si>
+    <t>{"messageType":"SplashG3Pool","result":{"pool":{"outRef":"dc3c6cbb319470b481ad65776619285268d96d02616d0c4f3d8863f714e2593d#3","address":"addr_test1xz7n46v3kk40ejh7tjnswk9ax65m97rj74lk6wsllg8twaaj764lvrxdayh2ux30fl0ktuh27csgmpevdu89jlxppvrs04w48j","coin":"5245194052","multiAssets":[{"policyId":"77359874a76d9cb19d4ae24c60e5e4d71ecde489584c3d0ff68091fe","assets":[{"name":"4144415f5553444d5f4e46545f32","value":"1"}]},{"policyId":"2863e0da31ab4fb792394b6ef9997c9235bdb7a64102dde9dd33d690","assets":[{"name":"4144415f5553444d5f4c515f32","value":"9223372033980443278"}]},{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"1327727217"}]}],"refScriptOutRef":"2b7efe0f19eedbb94abb4e505d87fac41143b9422792aafdf5927c3535b303d4#1","validityNft":"77359874a76d9cb19d4ae24c60e5e4d71ecde489584c3d0ff68091fe.4144415f5553444d5f4e46545f32","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","lpToken":"2863e0da31ab4fb792394b6ef9997c9235bdb7a64102dde9dd33d690.4144415f5553444d5f4c515f32","poolFee":91900,"treasuryFee":900,"royaltyFee":100,"treasuryA":"4707400","treasuryB":"1249221","royaltyA":"523038","royaltyB":"138797","daoPolicies":[],"treasuryAddressPkh":"75c4570eb625ae881b32a34c52b159f6f3f3f2c7aaabf5bac4688133","royaltyAddressPkh":"72c68f905716a5f59a0ee2552ab68559f42287d335396d8f430da98e96c5009c","royaltyNonce":"0"},"sequenceInfo":{"blockSlot":112590329,"transactionIndex":2},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:46:25.261</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"8b3c7c0ccd6e5bf57e2bc8663ce7bc63dc0f628136b0af10adb15a5c37b2f499#0","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vyuxcade0jfkhtz7e6mzqzw6c3a9r6h9mht3jt7mhe70sqq703vum","coin":"6755938856","multiAssets":[{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"15924768fc822a4b15df3b487738c41934f544dfc8aa6bfe692e2da39f7c4511","value":"1"}]},{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"2198947955"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.15924768fc822a4b15df3b487738c41934f544dfc8aa6bfe692e2da39f7c4511","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"17320508075688773","sqrtPriceLowerDen":"100000000000000000","sqrtPriceUpperNum":"9486832980505138","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":10,"platformFeeRate":500,"platformFeeA":"996398","platformFeeB":"388529","minTxAmountA":"39501417","minTxAmountB":"3093903","circulatingLpToken":"17313253216","lastWithdrawEpoch":67841,"stakingUtxo":{"outRef":"f7bf1318abd11ff715abda8fedf164690241941f4dcce6d963b6ac59dc862cfc#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113741131,"transactionIndex":2},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:46:25.262</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"f1f6c582b914a815b3287b305ec9839ec2d371733691a85ed07505fb187acda7#0","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vprnxs9yt369fqkyjq79t0qyzp5hrzn04cqlet4vhdsluzqwkehk0","coin":"1358774587","multiAssets":[{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"470437a5df9d8d3c4dc110d2f4f4d80d0082e6f68f91103fbc5412943423769e","value":"1"}]},{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"553048705"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.470437a5df9d8d3c4dc110d2f4f4d80d0082e6f68f91103fbc5412943423769e","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"1000000","sqrtPriceLowerDen":"10000000","sqrtPriceUpperNum":"9486832980505138","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":30,"platformFeeRate":500,"platformFeeA":"460207","platformFeeB":"144678","minTxAmountA":"37946489","minTxAmountB":"3220681","circulatingLpToken":"3241851765","lastWithdrawEpoch":67840,"stakingUtxo":{"outRef":"3f8a54141bfc7b46a245b8c487e9259433c198067de8ff16843cd67f0bfdd77a#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113739271,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:46:25.263</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"f9319731142fa79e551f321019ef788de6a45b246e71fae5c03e34b9e2dfc110#0","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vpd4pl6sta79ykcgxx065c3lycgwy9xm34vajm5x8vw6ldsde3rrc","coin":"43968250","multiAssets":[{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"147759273495"}]},{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"c4d966b065db0887d643f2992e82f8dc4782d0829ffaa3856998824037e710f9","value":"1"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.c4d966b065db0887d643f2992e82f8dc4782d0829ffaa3856998824037e710f9","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"24374579270728639","sqrtPriceLowerDen":"100000000000000000","sqrtPriceUpperNum":"33216952406275596","sqrtPriceUpperDen":"100000000000000000","poolFeeRate":10,"platformFeeRate":500,"platformFeeA":"927158","platformFeeB":"183865","minTxAmountA":"37946489","minTxAmountB":"3220681","circulatingLpToken":"701214764746","lastWithdrawEpoch":67839,"stakingUtxo":{"outRef":"02d4e9025876902fc2ee6c6b8e13f6a3ef444c8b6a89f8805833bb956415f832#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113736011,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:46:25.264</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"42179f276608e2f5655fc053f759db2e8047075232c5ff71aad76f2c018dc258#0","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vy2v94fpsddtn0xtkq4vj04sergmm5pz5pzcz6y82pvkzgqn89mn9","coin":"3014521","multiAssets":[{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"19991292"}]},{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"9a2e6155e399fd7f9e1810195b55f5730ff9b7b7280a094accb5e48ce0f2926a","value":"1"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.9a2e6155e399fd7f9e1810195b55f5730ff9b7b7280a094accb5e48ce0f2926a","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"23923183896578434","sqrtPriceLowerDen":"100000000000000000","sqrtPriceUpperNum":"32601804202361095","sqrtPriceUpperDen":"100000000000000000","poolFeeRate":10,"platformFeeRate":500,"platformFeeA":"14496","platformFeeB":"7532","minTxAmountA":"38662483","minTxAmountB":"3161037","circulatingLpToken":"97000000","lastWithdrawEpoch":67751,"stakingUtxo":{"outRef":"1178ae4595526868d0c0ed98d8aa470980370b9f4aa1be7c340b7fb67e8a5fb8#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113577895,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:46:25.265</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"d9302781869d6c7fb8cd8fd0e39a8de9a646b0467f4a5f890ad7c9f85157143c#2","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04v8yrwvdzwuumq0lcgphg2v357jnrwq876nezlt4349jcneq23lzrm","coin":"3090037","multiAssets":[{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"e57a5327ebc6c80248dd4fac8ce4c4bb318daf7bc2195a9ad59a21eccfe123d0","value":"1"}]},{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"57314714"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.e57a5327ebc6c80248dd4fac8ce4c4bb318daf7bc2195a9ad59a21eccfe123d0","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"20677736735999433","sqrtPriceLowerDen":"100000000000000000","sqrtPriceUpperNum":"2817900524149877","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":10,"platformFeeRate":500,"platformFeeA":"89518","platformFeeB":"7274","minTxAmountA":"44730703","minTxAmountB":"2732207","circulatingLpToken":"376108224","lastWithdrawEpoch":67700,"stakingUtxo":{"outRef":"62c21ad53ba10d49b57e2733cfc2f8f2461c743a3de3bd1bff5e6d9fd37ace3e#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113485666,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:46:25.266</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"d9302781869d6c7fb8cd8fd0e39a8de9a646b0467f4a5f890ad7c9f85157143c#1","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vx25zajjegptl98gtd6xs6uduuf5qqmtz6ekp0n8sltjc7q3gmyyy","coin":"3094131","multiAssets":[{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"60343161"}]},{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"d0c20b099ebdb52aba221386deda5f4930f9b72aa1221ccd2d0973a70d02badc","value":"1"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.d0c20b099ebdb52aba221386deda5f4930f9b72aa1221ccd2d0973a70d02badc","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"20677736735999433","sqrtPriceLowerDen":"100000000000000000","sqrtPriceUpperNum":"2817900524149877","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":10,"platformFeeRate":500,"platformFeeA":"93571","platformFeeB":"7579","minTxAmountA":"44730703","minTxAmountB":"2732207","circulatingLpToken":"397000000","lastWithdrawEpoch":67700,"stakingUtxo":{"outRef":"cfec8ec1e6c424afd9b724ba58552c5f781e83fc6df3fa73996c5960dd88c321#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113485666,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:46:25.267</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"d044ce73aa3738f746b3772336e9b4ea4920c3c8dc7242f55cf31600d932f7a8#0","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vyunnxqnevxe0ufjaxmwyakld723canz56wg2prqh2n27us3506ft","coin":"3034201","multiAssets":[{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"14942308"}]},{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"26f11dbf94cf846cb34cc0572b857ffc626adf61c42d0b60a549d67f09431758","value":"1"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.26f11dbf94cf846cb34cc0572b857ffc626adf61c42d0b60a549d67f09431758","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"20677736735999433","sqrtPriceLowerDen":"100000000000000000","sqrtPriceUpperNum":"2817900524149877","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":10,"platformFeeRate":500,"platformFeeA":"34199","platformFeeB":"3006","minTxAmountA":"44730703","minTxAmountB":"2732207","circulatingLpToken":"97000000","lastWithdrawEpoch":67551,"stakingUtxo":{"outRef":"f9c82a78645d57d4afcdec482fe5b9fc2565da53e511614109484b2836c14cbe#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113218427,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:46:25.292</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"b8b6da0c452545db7b60d0499ef00202af78a6c14f61052373e9a7c3fcb7e33f#2","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vqdax6vmwwwj6wcj2yzqpjs7thun50vxynuh0vpfy3zzegqsjka7n","coin":"3000008","multiAssets":[{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"7108752"}]},{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"3126f6b928ae5aa7dc25d82d98a6fd8ed8fdce26885481e84f7bd358583d93af","value":"1"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.3126f6b928ae5aa7dc25d82d98a6fd8ed8fdce26885481e84f7bd358583d93af","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"21520116174491596","sqrtPriceLowerDen":"100000000000000000","sqrtPriceUpperNum":"29326974911277726","sqrtPriceUpperDen":"100000000000000000","poolFeeRate":10,"platformFeeRate":500,"platformFeeA":"0","platformFeeB":"158","minTxAmountA":"42979773","minTxAmountB":"2843513","circulatingLpToken":"41795764","lastWithdrawEpoch":67299,"stakingUtxo":{"outRef":"b450aacb59445d0081d994f828608769053fc0f8aa4bcdaa889803719bebd049#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":112765522,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:46:25.294</t>
+  </si>
+  <si>
+    <t>scribeDexEvent","params":{"type":"nioblockchain.tradingaggregator.model.DexEvent","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d"}}</t>
+  </si>
+  <si>
+    <t>17:44:58.655</t>
+  </si>
+  <si>
+    <t>swap 60</t>
+  </si>
+  <si>
+    <t>https://preprod.cardanoscan.io/transaction/8b3c7c0ccd6e5bf57e2bc8663ce7bc63dc0f628136b0af10adb15a5c37b2f499</t>
+  </si>
+  <si>
+    <t>17:44:58.663</t>
+  </si>
+  <si>
+    <t>17:44:58.668</t>
+  </si>
+  <si>
+    <t>17:44:58.669</t>
+  </si>
+  <si>
+    <t>17:44:58.670</t>
+  </si>
+  <si>
+    <t>17:44:58.672</t>
+  </si>
+  <si>
+    <t>17:44:58.674</t>
+  </si>
+  <si>
+    <t>17:44:58.675</t>
+  </si>
+  <si>
+    <t>17:44:58.677</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"f1f6c582b914a815b3287b305ec9839ec2d371733691a85ed07505fb187acda7#1","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vyuxcade0jfkhtz7e6mzqzw6c3a9r6h9mht3jt7mhe70sqq703vum","coin":"6695938859","multiAssets":[{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"2213514560"}]},{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"15924768fc822a4b15df3b487738c41934f544dfc8aa6bfe692e2da39f7c4511","value":"1"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.15924768fc822a4b15df3b487738c41934f544dfc8aa6bfe692e2da39f7c4511","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"17320508075688773","sqrtPriceLowerDen":"100000000000000000","sqrtPriceUpperNum":"9486832980505138","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":10,"platformFeeRate":500,"platformFeeA":"993399","platformFeeB":"388529","minTxAmountA":"39501417","minTxAmountB":"3093903","circulatingLpToken":"17313253216","lastWithdrawEpoch":67840,"stakingUtxo":{"outRef":"f7bf1318abd11ff715abda8fedf164690241941f4dcce6d963b6ac59dc862cfc#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113739271,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:44:58.678</t>
+  </si>
+  <si>
+    <t>17:44:58.679</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"e540c1822cf6e1d7f4cc4f0bcea5c879a60d081ab58db72c7eedf98ce4593320#0","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vprnxs9yt369fqkyjq79t0qyzp5hrzn04cqlet4vhdsluzqwkehk0","coin":"1202457095","multiAssets":[{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"470437a5df9d8d3c4dc110d2f4f4d80d0082e6f68f91103fbc5412943423769e","value":"1"}]},{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"593414336"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.470437a5df9d8d3c4dc110d2f4f4d80d0082e6f68f91103fbc5412943423769e","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"1000000","sqrtPriceLowerDen":"10000000","sqrtPriceUpperNum":"9486832980505138","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":30,"platformFeeRate":500,"platformFeeA":"436760","platformFeeB":"144678","minTxAmountA":"37946489","minTxAmountB":"3220681","circulatingLpToken":"3241851765","lastWithdrawEpoch":67839,"stakingUtxo":{"outRef":"3f8a54141bfc7b46a245b8c487e9259433c198067de8ff16843cd67f0bfdd77a#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113736442,"transactionIndex":4},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>17:12:53.855</t>
+  </si>
+  <si>
+    <t>17:12:53.858</t>
+  </si>
+  <si>
+    <t>17:12:53.859</t>
+  </si>
+  <si>
+    <t>17:12:53.860</t>
+  </si>
+  <si>
+    <t>17:12:53.862</t>
+  </si>
+  <si>
+    <t>17:12:53.863</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"e68462cc1745c862d1629e36447f5917231cbc00373925eeebdb60ef4dea9b49#1","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vyuxcade0jfkhtz7e6mzqzw6c3a9r6h9mht3jt7mhe70sqq703vum","coin":"5952256355","multiAssets":[{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"2405040085"}]},{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"15924768fc822a4b15df3b487738c41934f544dfc8aa6bfe692e2da39f7c4511","value":"1"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.15924768fc822a4b15df3b487738c41934f544dfc8aa6bfe692e2da39f7c4511","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"17320508075688773","sqrtPriceLowerDen":"100000000000000000","sqrtPriceUpperNum":"9486832980505138","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":10,"platformFeeRate":500,"platformFeeA":"956215","platformFeeB":"388529","minTxAmountA":"39501417","minTxAmountB":"3093903","circulatingLpToken":"17313253216","lastWithdrawEpoch":67839,"stakingUtxo":{"outRef":"f7bf1318abd11ff715abda8fedf164690241941f4dcce6d963b6ac59dc862cfc#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113735878,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>{"messageType":"SplashG3Pool","result":{"pool":{"outRef":"01e111fb2701dc46a402a15d1828e91f874a6a54969fe30d095c534a23c67f4e#0","address":"addr_test1xz7n46v3kk40ejh7tjnswk9ax65m97rj74lk6wsllg8twaaj764lvrxdayh2ux30fl0ktuh27csgmpevdu89jlxppvrs04w48j","coin":"567913280861","multiAssets":[{"policyId":"82fdffb1016939f6d0c2a27b2393aafb6e310127c46fed48f664dc11","assets":[{"name":"665553444d5f4144415f4e4654","value":"1"}]},{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"146509536163"}]},{"policyId":"494926363f11ae6413e48ab65d8b3e6730e1e278991285547dbb391d","assets":[{"name":"665553444d5f4144415f4c51","value":"9223371753596942730"}]}],"refScriptOutRef":"2b7efe0f19eedbb94abb4e505d87fac41143b9422792aafdf5927c3535b303d4#1","validityNft":"82fdffb1016939f6d0c2a27b2393aafb6e310127c46fed48f664dc11.665553444d5f4144415f4e4654","tokenA":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","tokenB":"","lpToken":"494926363f11ae6413e48ab65d8b3e6730e1e278991285547dbb391d.665553444d5f4144415f4c51","poolFee":99100,"treasuryFee":50,"royaltyFee":50,"treasuryA":"163566432","treasuryB":"438378405","royaltyA":"163566432","royaltyB":"438378405","daoPolicies":[],"treasuryAddressPkh":"75c4570eb625ae881b32a34c52b159f6f3f3f2c7aaabf5bac4688133","royaltyAddressPkh":"72c68f905716a5f59a0ee2552ab68559f42287d335396d8f430da98e96c5009c","royaltyNonce":"0"},"sequenceInfo":{"blockSlot":113733421,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"33f64acf242f40f4b29788d2d881715651c8912b4e95736abd8a326ab43182c0#0","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vyuxcade0jfkhtz7e6mzqzw6c3a9r6h9mht3jt7mhe70sqq703vum","coin":"5993957834","multiAssets":[{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"2393650935"}]},{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"15924768fc822a4b15df3b487738c41934f544dfc8aa6bfe692e2da39f7c4511","value":"1"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.15924768fc822a4b15df3b487738c41934f544dfc8aa6bfe692e2da39f7c4511","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"17320508075688773","sqrtPriceLowerDen":"100000000000000000","sqrtPriceUpperNum":"9486832980505138","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":10,"platformFeeRate":500,"platformFeeA":"950716","platformFeeB":"386486","minTxAmountA":"39501417","minTxAmountB":"3093903","circulatingLpToken":"17313253216","lastWithdrawEpoch":67836,"stakingUtxo":{"outRef":"f7bf1318abd11ff715abda8fedf164690241941f4dcce6d963b6ac59dc862cfc#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113731275,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"0f076bba482cc43312251678a23339ac94cffd3b60606a0b05c123659568cf28#0","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vprnxs9yt369fqkyjq79t0qyzp5hrzn04cqlet4vhdsluzqwkehk0","coin":"1162457095","multiAssets":[{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"573622523"}]},{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"470437a5df9d8d3c4dc110d2f4f4d80d0082e6f68f91103fbc5412943423769e","value":"1"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.470437a5df9d8d3c4dc110d2f4f4d80d0082e6f68f91103fbc5412943423769e","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"1000000","sqrtPriceLowerDen":"10000000","sqrtPriceUpperNum":"9486832980505138","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":30,"platformFeeRate":500,"platformFeeA":"436760","platformFeeB":"144678","minTxAmountA":"37946489","minTxAmountB":"3220681","circulatingLpToken":"3133701748","lastWithdrawEpoch":67830,"stakingUtxo":{"outRef":"3f8a54141bfc7b46a245b8c487e9259433c198067de8ff16843cd67f0bfdd77a#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113720127,"transactionIndex":1},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"bc9bed218b461a69e31118a6d1afa0b839371d18b277d9e2e592a87602f275fb#0","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vpd4pl6sta79ykcgxx065c3lycgwy9xm34vajm5x8vw6ldsde3rrc","coin":"3968251","multiAssets":[{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"147763682510"}]},{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"c4d966b065db0887d643f2992e82f8dc4782d0829ffaa3856998824037e710f9","value":"1"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.c4d966b065db0887d643f2992e82f8dc4782d0829ffaa3856998824037e710f9","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"24374579270728639","sqrtPriceLowerDen":"100000000000000000","sqrtPriceUpperNum":"33216952406275596","sqrtPriceUpperDen":"100000000000000000","poolFeeRate":10,"platformFeeRate":500,"platformFeeA":"925159","platformFeeB":"183865","minTxAmountA":"37946489","minTxAmountB":"3220681","circulatingLpToken":"701214764746","lastWithdrawEpoch":67799,"stakingUtxo":{"outRef":"02d4e9025876902fc2ee6c6b8e13f6a3ef444c8b6a89f8805833bb956415f832#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113664343,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>{"messageType":"SplashG3Pool","result":{"pool":{"outRef":"b721e1d78a4e3e58cb13a42b425bba08691350458a5522d19d8fa737eb47d692#1","address":"addr_test1xz7n46v3kk40ejh7tjnswk9ax65m97rj74lk6wsllg8twaaj764lvrxdayh2ux30fl0ktuh27csgmpevdu89jlxppvrs04w48j","coin":"569234536030","multiAssets":[{"policyId":"82fdffb1016939f6d0c2a27b2393aafb6e310127c46fed48f664dc11","assets":[{"name":"665553444d5f4144415f4e4654","value":"1"}]},{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"146166282156"}]},{"policyId":"494926363f11ae6413e48ab65d8b3e6730e1e278991285547dbb391d","assets":[{"name":"665553444d5f4144415f4c51","value":"9223371753596942730"}]}],"refScriptOutRef":"2b7efe0f19eedbb94abb4e505d87fac41143b9422792aafdf5927c3535b303d4#1","validityNft":"82fdffb1016939f6d0c2a27b2393aafb6e310127c46fed48f664dc11.665553444d5f4144415f4e4654","tokenA":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","tokenB":"","lpToken":"494926363f11ae6413e48ab65d8b3e6730e1e278991285547dbb391d.665553444d5f4144415f4c51","poolFee":99100,"treasuryFee":50,"royaltyFee":50,"treasuryA":"163394805","treasuryB":"438378405","royaltyA":"163394805","royaltyB":"438378405","daoPolicies":[],"treasuryAddressPkh":"75c4570eb625ae881b32a34c52b159f6f3f3f2c7aaabf5bac4688133","royaltyAddressPkh":"72c68f905716a5f59a0ee2552ab68559f42287d335396d8f430da98e96c5009c","royaltyNonce":"0"},"sequenceInfo":{"blockSlot":113732381,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>15:36:04.925</t>
+  </si>
+  <si>
+    <t>15:36:04.929</t>
+  </si>
+  <si>
+    <t>15:36:04.930</t>
+  </si>
+  <si>
+    <t>15:36:04.931</t>
+  </si>
+  <si>
+    <t>15:36:04.933</t>
+  </si>
+  <si>
+    <t>15:36:04.934</t>
+  </si>
+  <si>
+    <t>15:36:04.935</t>
+  </si>
+  <si>
+    <t>15:36:04.936</t>
+  </si>
+  <si>
+    <t>15:36:04.937</t>
+  </si>
+  <si>
+    <t>15:36:04.938</t>
+  </si>
+  <si>
+    <t>15:36:04.940</t>
+  </si>
+  <si>
     <t>{"messageType":"SplashG3Pool","result":{"pool":{"outRef":"fb9734d6f0469987d741eac6708080c1d5d9f89dcbaca79e7c3331c7199962c1#0","address":"addr_test1xz7n46v3kk40ejh7tjnswk9ax65m97rj74lk6wsllg8twaaj764lvrxdayh2ux30fl0ktuh27csgmpevdu89jlxppvrs04w48j","coin":"573264120626","multiAssets":[{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"145124950294"}]},{"policyId":"494926363f11ae6413e48ab65d8b3e6730e1e278991285547dbb391d","assets":[{"name":"665553444d5f4144415f4c51","value":"9223371753596942730"}]},{"policyId":"82fdffb1016939f6d0c2a27b2393aafb6e310127c46fed48f664dc11","assets":[{"name":"665553444d5f4144415f4e4654","value":"1"}]}],"refScriptOutRef":"2b7efe0f19eedbb94abb4e505d87fac41143b9422792aafdf5927c3535b303d4#1","validityNft":"82fdffb1016939f6d0c2a27b2393aafb6e310127c46fed48f664dc11.665553444d5f4144415f4e4654","tokenA":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","tokenB":"","lpToken":"494926363f11ae6413e48ab65d8b3e6730e1e278991285547dbb391d.665553444d5f4144415f4c51","poolFee":99100,"treasuryFee":50,"royaltyFee":50,"treasuryA":"162767502","treasuryB":"437957030","royaltyA":"162767502","royaltyB":"437957030","daoPolicies":[],"treasuryAddressPkh":"75c4570eb625ae881b32a34c52b159f6f3f3f2c7aaabf5bac4688133","royaltyAddressPkh":"72c68f905716a5f59a0ee2552ab68559f42287d335396d8f430da98e96c5009c","royaltyNonce":"0"},"sequenceInfo":{"blockSlot":112845554,"transactionIndex":0}}}</t>
   </si>
   <si>
@@ -127,6 +480,51 @@
     <t>17:31:57.762</t>
   </si>
   <si>
+    <t>{"messageType":"SplashG3Pool","result":{"pool":{"outRef":"8e11f60a78f9fa0d7cbdc4582f1d6ee4ba4d8cf150176fe38c9ca12fc831aef5#0","address":"addr_test1xz7n46v3kk40ejh7tjnswk9ax65m97rj74lk6wsllg8twaaj764lvrxdayh2ux30fl0ktuh27csgmpevdu89jlxppvrs04w48j","coin":"569633950720","multiAssets":[{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"146062831093"}]},{"policyId":"82fdffb1016939f6d0c2a27b2393aafb6e310127c46fed48f664dc11","assets":[{"name":"665553444d5f4144415f4e4654","value":"1"}]},{"policyId":"494926363f11ae6413e48ab65d8b3e6730e1e278991285547dbb391d","assets":[{"name":"665553444d5f4144415f4c51","value":"9223371753596942730"}]}],"refScriptOutRef":"2b7efe0f19eedbb94abb4e505d87fac41143b9422792aafdf5927c3535b303d4#1","validityNft":"82fdffb1016939f6d0c2a27b2393aafb6e310127c46fed48f664dc11.665553444d5f4144415f4e4654","tokenA":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","tokenB":"","lpToken":"494926363f11ae6413e48ab65d8b3e6730e1e278991285547dbb391d.665553444d5f4144415f4c51","poolFee":99100,"treasuryFee":50,"royaltyFee":50,"treasuryA":"163343081","treasuryB":"438378405","royaltyA":"163343081","royaltyB":"438378405","daoPolicies":[],"treasuryAddressPkh":"75c4570eb625ae881b32a34c52b159f6f3f3f2c7aaabf5bac4688133","royaltyAddressPkh":"72c68f905716a5f59a0ee2552ab68559f42287d335396d8f430da98e96c5009c","royaltyNonce":"0"},"sequenceInfo":{"blockSlot":113394158,"transactionIndex":2},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>13:41:47.609</t>
+  </si>
+  <si>
+    <t>13:41:47.611</t>
+  </si>
+  <si>
+    <t>13:41:47.612</t>
+  </si>
+  <si>
+    <t>13:41:47.613</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"0f076bba482cc43312251678a23339ac94cffd3b60606a0b05c123659568cf28#1","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04vyuxcade0jfkhtz7e6mzqzw6c3a9r6h9mht3jt7mhe70sqq703vum","coin":"5895280978","multiAssets":[{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"15924768fc822a4b15df3b487738c41934f544dfc8aa6bfe692e2da39f7c4511","value":"1"}]},{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"2420523063"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.15924768fc822a4b15df3b487738c41934f544dfc8aa6bfe692e2da39f7c4511","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"17320508075688773","sqrtPriceLowerDen":"100000000000000000","sqrtPriceUpperNum":"9486832980505138","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":10,"platformFeeRate":500,"platformFeeA":"945717","platformFeeB":"386486","minTxAmountA":"39501417","minTxAmountB":"3093903","circulatingLpToken":"17313253216","lastWithdrawEpoch":67830,"stakingUtxo":{"outRef":"f7bf1318abd11ff715abda8fedf164690241941f4dcce6d963b6ac59dc862cfc#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113720127,"transactionIndex":1},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>13:41:47.614</t>
+  </si>
+  <si>
+    <t>13:41:47.615</t>
+  </si>
+  <si>
+    <t>13:41:47.674</t>
+  </si>
+  <si>
+    <t>{"messageType":"ConcentratedPool","result":{"pool":{"outRef":"d9302781869d6c7fb8cd8fd0e39a8de9a646b0467f4a5f890ad7c9f85157143c#2","address":"addr_test1xqnn54m2thnffl6swaju2768alwgr6nlzwjrm3zyzez04v8yrwvdzwuumq0lcgphg2v357jnrwq876nezlt4349jcneq23lzrm","coin":"3090037","multiAssets":[{"policyId":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905","assets":[{"name":"665553444d","value":"57314714"}]},{"policyId":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0","assets":[{"name":"e57a5327ebc6c80248dd4fac8ce4c4bb318daf7bc2195a9ad59a21eccfe123d0","value":"1"}]}],"refScriptOutRef":"14c60e738ba8296ee46abf2546a8234cb899f38f4ca410f3274ab9c7e38d032b#0","validityNft":"273a576a5de694ff507765c57b47efdc81ea7f13a43dc4441644fab0.e57a5327ebc6c80248dd4fac8ce4c4bb318daf7bc2195a9ad59a21eccfe123d0","tokenA":"","tokenB":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","sqrtPriceLowerNum":"20677736735999433","sqrtPriceLowerDen":"100000000000000000","sqrtPriceUpperNum":"2817900524149877","sqrtPriceUpperDen":"10000000000000000","poolFeeRate":10,"platformFeeRate":500,"platformFeeA":"89518","platformFeeB":"7274","minTxAmountA":"44730703","minTxAmountB":"2732207","circulatingLpToken":"376108224","lastWithdrawEpoch":67700,"stakingUtxo":{"outRef":"62c21ad53ba10d49b57e2733cfc2f8f2461c743a3de3bd1bff5e6d9fd37ace3e#1","rewardAmount":"0"}},"sequenceInfo":{"blockSlot":113485666,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>13:41:47.676</t>
+  </si>
+  <si>
+    <t>13:41:47.678</t>
+  </si>
+  <si>
+    <t>{"messageType":"FloatPool","result":{"pool":{"outRef":"fadb531433d3d4b4431d3855b6889c2dae07cb0ff7ed0e1577a40878d6bc499a#1","address":"addr_test1wp4nhp3neyyd0hqhq92a5v3aqqytldmdtcfrry3kpqcv4rgt8arjt","coin":"5000000","multiAssets":[{"policyId":"703d581d9a657d1326aea6a754cdcf191efb22133a62a181951156cf","assets":[{"name":"","value":"62680719607"}]},{"policyId":"e5e9120138ff062befc0b55f840dc632e4ccac51740600d78403273a","assets":[{"name":"435a1f498bf490359a86e94918cb09806d9c28d85d0b44659061ff4a","value":"1"}]}],"poolId":"e5e9120138ff062befc0b55f840dc632e4ccac51740600d78403273a.435a1f498bf490359a86e94918cb09806d9c28d85d0b44659061ff4a","dToken":"6b3b8633c908d7dc170155da323d0008bfb76d5e123192360830ca8d.435a1f498bf490359a86e94918cb09806d9c28d85d0b44659061ff4a","totalSupply":"276820137960","circulatingDToken":"262627842695","totalBorrow":"212900973853","borrowApy":969,"undistributedFee":"5651592","interestIndex":"1193876509015","interestTime":"1769163685000","alternativeSupplyTokens":[{"latestExchangeRateNum":"64213874086","latestExchangeRateDen":"62964151614"}]},"marketToken":"","sequenceInfo":{"blockSlot":113480603,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>{"messageType":"OraclePath","result":{"oraclePath":{"baseToken":"","quoteToken":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","globalConfigOutRef":"95027d0239652d5ac47cf901eb44a322bf317da7a14a1adb8404deb5ee7f3a19#0","oraclePathOutRef":"d8935573cd02d5bbd92fb371c3386d752b222a71e462ea7b3d3bfb935435f67c#0","pricePaths":[[{"oracleType":"SPLASH_POOL","isReversed":true,"priceOption":"A_PER_B","validityNft":"82fdffb1016939f6d0c2a27b2393aafb6e310127c46fed48f664dc11.665553444d5f4144415f4e4654"}]],"priceDeviationThreshold":500},"sequenceInfo":{"blockSlot":113296648,"transactionIndex":0},"isSpent":false}}</t>
+  </si>
+  <si>
+    <t>13:41:47.681</t>
+  </si>
+  <si>
     <t>{"method":"subscribeDexEvent","params":{"type":"nioblockchain.tradingaggregator.model.DexEvent","tokenA":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","tokenB":""}}</t>
   </si>
   <si>
@@ -217,16 +615,10 @@
     <t>15:20:21.858</t>
   </si>
   <si>
-    <t>{"method":"subscribeOracleEvent","params":{"type":"nioblockchain.tradingaggregator.model.OracleEvent","tokenPairs":[{"baseToken":"703d581d9a657d1326aea6a754cdcf191efb22133a62a181951156cf","quoteToken":""}]}}</t>
-  </si>
-  <si>
     <t>15:20:21.860</t>
   </si>
   <si>
     <t>{"messageType":"FloatPoolParam","result":{"poolParam":{"outRef":"befd26008b6a967a9ad480611100c5e01bd82ef0437648cd563c76e6f5db2273#0","address":"addr_test1wrj7jysp8rlsv2l0cz64lpqdccewfn9v296qvqxhsspjwwslx7k0s","coin":"2086040","multiAssets":[{"policyId":"e5e9120138ff062befc0b55f840dc632e4ccac51740600d78403273a","assets":[{"name":"520aa368b4b171ee9de426e3e1ff568b1f5cf77d77f97ef7066bcb59","value":"1"}]}],"poolId":"e5e9120138ff062befc0b55f840dc632e4ccac51740600d78403273a.520aa368b4b171ee9de426e3e1ff568b1f5cf77d77f97ef7066bcb59","baseInterestRate":100,"powerBase":10200,"minTxAmount":"99","utilizationCap":9000,"loanFeeRate":1000,"loanOriginationFeeRate":0,"withdrawalFee":"0","loanOriginationFeeMinAmount":"0","feeAddress":"addr_test1qr20zc2v0fyxwjf42jy8vjctfpqrc9f3md3cwe6fccsza9g5q42ut28rqch23fj0j4hp479jdkeyn2mpv8tmxk3h5jeqsm9xmy","liquidatorRewardCap":1000,"collectorReward":"0","supportedCollaterals":[{"token":"","liquidationThreshold":8000,"minSupplyAmount":"0","isEnable":true},{"token":"834a15101873b4e1ddfaa830df46792913995d8738dcde34eda27905.665553444d","liquidationThreshold":8000,"minSupplyAmount":"0","isEnable":true},{"token":"9a614be30284aa88eb845da7657b5d0a235f1b95628b23c08050d502.6655534441","liquidationThreshold":6000,"minSupplyAmount":"0","isEnable":true}],"alternativeSupplyTokens":[]},"marketToken":"","sequenceInfo":{"blockSlot":103184845,"transactionIndex":0}}}</t>
-  </si>
-  <si>
-    <t>{"method":"subscribeOracleEvent","params":{"type":"nioblockchain.tradingaggregator.model.OracleEvent","tokenPairs":[{"baseToken":"","quoteToken":""}]}}</t>
   </si>
   <si>
     <t>15:20:21.861</t>
@@ -713,7 +1105,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -752,6 +1144,37 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFCE27C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDEC663"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFCE27C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFCE27C"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFCE27C"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -875,13 +1298,13 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -908,16 +1331,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -926,19 +1349,19 @@
     <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1002,7 +1425,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1042,37 +1465,76 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1143,6 +1605,288 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>6200775</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2514600"/>
+          <a:ext cx="6200775" cy="4429125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>5543550</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1371600"/>
+          <a:ext cx="5543550" cy="4267200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>5248275</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2895600"/>
+          <a:ext cx="5248275" cy="4867275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>5172075</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3048000"/>
+          <a:ext cx="5172075" cy="4514850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4886325</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3810000"/>
+          <a:ext cx="4886325" cy="7334250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4762500"/>
+          <a:ext cx="8353425" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1403,10 +2147,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1419,245 +2163,494 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" ht="15.75" spans="1:4">
+      <c r="A2" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="29">
+        <v>1304</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="28"/>
+    </row>
+    <row r="3" ht="15.75" spans="1:4">
+      <c r="A3" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="32">
+        <v>1491</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="31"/>
+    </row>
+    <row r="4" ht="15.75" spans="1:4">
+      <c r="A4" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="32">
+        <v>1486</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="31"/>
+    </row>
+    <row r="5" ht="15.75" spans="1:4">
+      <c r="A5" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="32">
+        <v>1487</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="31"/>
+    </row>
+    <row r="6" ht="15.75" spans="1:4">
+      <c r="A6" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="32">
+        <v>1442</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="31"/>
+    </row>
+    <row r="7" ht="15.75" spans="1:4">
+      <c r="A7" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="32">
+        <v>1439</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="31"/>
+    </row>
+    <row r="8" ht="15.75" spans="1:4">
+      <c r="A8" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="32">
+        <v>1455</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="31"/>
+    </row>
+    <row r="9" ht="15.75" spans="1:4">
+      <c r="A9" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="32">
+        <v>1452</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="31"/>
+    </row>
+    <row r="10" ht="15.75" spans="1:4">
+      <c r="A10" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="32">
+        <v>1428</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="31"/>
+    </row>
+    <row r="11" ht="15.75" spans="1:4">
+      <c r="A11" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="32">
+        <v>1441</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="31"/>
+    </row>
+    <row r="12" ht="15.75" spans="1:4">
+      <c r="A12" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="32">
+        <v>1441</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="31"/>
+    </row>
+    <row r="13" ht="15.75" spans="1:4">
+      <c r="A13" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="32">
+        <v>1440</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="31"/>
+    </row>
+    <row r="14" ht="15.75" spans="1:4">
+      <c r="A14" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="32">
+        <v>1137</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="31"/>
+    </row>
+    <row r="15" ht="15.75" spans="1:4">
+      <c r="A15" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="32">
+        <v>1159</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="31"/>
+    </row>
+    <row r="16" ht="15.75" spans="1:4">
+      <c r="A16" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="32">
+        <v>931</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="31"/>
+    </row>
+    <row r="17" ht="15.75" spans="1:4">
+      <c r="A17" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="32">
+        <v>3539</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="31"/>
+    </row>
+    <row r="18" ht="15.75" spans="1:4">
+      <c r="A18" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="35">
+        <v>207</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="34"/>
+    </row>
+    <row r="19" ht="15.75" spans="1:4">
+      <c r="A19" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="32">
+        <v>1405</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="31"/>
+    </row>
+    <row r="20" ht="15.75" spans="1:2">
+      <c r="A20" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="35">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="C33:D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="119.428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="14">
+      <c r="A2" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="20">
         <v>1475</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="16"/>
+      <c r="C2" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="25"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="17">
+      <c r="A3" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="23">
         <v>1470</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="13"/>
+      <c r="C3" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="17">
+      <c r="A4" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="23">
         <v>1471</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="13"/>
+      <c r="C4" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="19">
+      <c r="A5" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="14">
         <v>1431</v>
       </c>
-      <c r="C5" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="21"/>
+      <c r="C5" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="13"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="22">
+      <c r="A6" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="17">
         <v>1408</v>
       </c>
-      <c r="C6" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="13"/>
+      <c r="C6" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="16"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="22">
+      <c r="A7" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="17">
         <v>1424</v>
       </c>
-      <c r="C7" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="13"/>
+      <c r="C7" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="22">
+      <c r="A8" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="17">
         <v>1424</v>
       </c>
-      <c r="C8" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="13"/>
+      <c r="C8" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="16"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="22">
+      <c r="A9" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" s="17">
         <v>1422</v>
       </c>
-      <c r="C9" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="13"/>
+      <c r="C9" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" s="16"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="22">
+      <c r="A10" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" s="17">
         <v>1421</v>
       </c>
-      <c r="C10" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="13"/>
+      <c r="C10" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" s="16"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="22">
+      <c r="A11" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B11" s="17">
         <v>1398</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="13"/>
+      <c r="C11" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="22">
+      <c r="A12" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" s="17">
         <v>1300</v>
       </c>
-      <c r="C12" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="13"/>
+      <c r="C12" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="16"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="22">
+      <c r="A13" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13" s="17">
         <v>1396</v>
       </c>
-      <c r="C13" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="13"/>
+      <c r="C13" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="D13" s="16"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="22">
+      <c r="A14" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="17">
         <v>1424</v>
       </c>
-      <c r="C14" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="13"/>
+      <c r="C14" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="D14" s="16"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="22">
+      <c r="A15" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" s="17">
         <v>1398</v>
       </c>
-      <c r="C15" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="13"/>
+      <c r="C15" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="D15" s="16"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="22">
+      <c r="A16" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16" s="17">
         <v>1396</v>
       </c>
-      <c r="C16" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="13"/>
+      <c r="C16" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="D16" s="16"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="22">
+      <c r="A17" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" s="17">
         <v>1419</v>
       </c>
-      <c r="C17" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="13"/>
+      <c r="C17" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="D17" s="16"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="22">
+      <c r="A18" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" s="17">
         <v>1420</v>
       </c>
-      <c r="C18" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="13"/>
+      <c r="C18" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="D18" s="16"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="22">
+      <c r="A19" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B19" s="17">
         <v>1303</v>
       </c>
-      <c r="C19" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="13"/>
+      <c r="C19" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="22">
+      <c r="A20" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" s="17">
         <v>1430</v>
       </c>
-      <c r="C20" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="13"/>
+      <c r="C20" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="D20" s="16"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="22">
+      <c r="A21" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B21" s="17">
         <v>1419</v>
       </c>
-      <c r="C21" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="13"/>
+      <c r="C21" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D21" s="16"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A21">
@@ -1668,7 +2661,467 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="C33:D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="119.428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="14">
+        <v>1491</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="17">
+        <v>1486</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="17">
+        <v>1487</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="17">
+        <v>1439</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="17">
+        <v>1435</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="17">
+        <v>1428</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="17">
+        <v>1450</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="17">
+        <v>1452</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="17">
+        <v>1441</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="B11" s="17">
+        <v>1440</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="D11" s="16"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="17">
+        <v>1440</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="D12" s="16"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="17">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="B14" s="17">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" s="20">
+        <v>624</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="D15" s="19"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" s="23">
+        <v>1491</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="D16" s="22"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="22"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="22"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="16"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="16"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="16"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="16"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A18:A21">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="C33:D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="119.428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="14">
+        <v>1491</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="17">
+        <v>1486</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="17">
+        <v>1487</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="17">
+        <v>1439</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="17">
+        <v>1435</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="17">
+        <v>1428</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="17">
+        <v>1450</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="17">
+        <v>1452</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="17">
+        <v>1441</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="B11" s="17">
+        <v>1440</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="D11" s="16"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="17">
+        <v>1440</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="D12" s="16"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="17">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="B14" s="17">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" s="20">
+        <v>624</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="D15" s="19"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" s="23">
+        <v>1491</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="D16" s="22"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="22"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="22"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="16"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="16"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="16"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="16"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A18:A21">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:D35"/>
@@ -1689,211 +3142,211 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="9" t="s">
-        <v>36</v>
+        <v>165</v>
       </c>
       <c r="B2" s="10">
         <v>188</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>37</v>
+        <v>166</v>
       </c>
       <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>38</v>
+        <v>167</v>
       </c>
       <c r="B3" s="8">
         <v>130</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>37</v>
+        <v>166</v>
       </c>
       <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>39</v>
+        <v>168</v>
       </c>
       <c r="B4" s="8">
         <v>218</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>37</v>
+        <v>166</v>
       </c>
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>3</v>
+        <v>117</v>
       </c>
       <c r="B5" s="5">
         <v>1470</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>40</v>
+        <v>169</v>
       </c>
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>5</v>
+        <v>119</v>
       </c>
       <c r="B6" s="5">
         <v>1471</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>41</v>
+        <v>170</v>
       </c>
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>1</v>
+        <v>115</v>
       </c>
       <c r="B7" s="5">
         <v>1475</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>42</v>
+        <v>171</v>
       </c>
       <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>32</v>
+        <v>146</v>
       </c>
       <c r="B8" s="5">
         <v>1430</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>43</v>
+        <v>172</v>
       </c>
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>34</v>
+        <v>148</v>
       </c>
       <c r="B9" s="5">
         <v>1419</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>44</v>
+        <v>173</v>
       </c>
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>27</v>
+        <v>141</v>
       </c>
       <c r="B10" s="5">
         <v>1419</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>45</v>
+        <v>174</v>
       </c>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="4" t="s">
-        <v>29</v>
+        <v>143</v>
       </c>
       <c r="B11" s="5">
         <v>1420</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>46</v>
+        <v>175</v>
       </c>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="4" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
       <c r="B12" s="5">
         <v>1303</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>47</v>
+        <v>176</v>
       </c>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="4" t="s">
-        <v>12</v>
+        <v>126</v>
       </c>
       <c r="B13" s="5">
         <v>1424</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>48</v>
+        <v>177</v>
       </c>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="4" t="s">
-        <v>49</v>
+        <v>178</v>
       </c>
       <c r="B14" s="5">
         <v>1431</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>50</v>
+        <v>179</v>
       </c>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="4" t="s">
-        <v>8</v>
+        <v>122</v>
       </c>
       <c r="B15" s="5">
         <v>1408</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>51</v>
+        <v>180</v>
       </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="4" t="s">
-        <v>10</v>
+        <v>124</v>
       </c>
       <c r="B16" s="5">
         <v>1424</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>52</v>
+        <v>181</v>
       </c>
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="4" t="s">
-        <v>16</v>
+        <v>130</v>
       </c>
       <c r="B17" s="5">
         <v>1421</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>53</v>
+        <v>182</v>
       </c>
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
-        <v>23</v>
+        <v>137</v>
       </c>
       <c r="B18" s="5">
         <v>1424</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>54</v>
+        <v>183</v>
       </c>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="7" t="s">
-        <v>24</v>
+        <v>138</v>
       </c>
       <c r="B19" s="8">
         <v>1398</v>
@@ -1901,187 +3354,187 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="9" t="s">
-        <v>26</v>
+        <v>140</v>
       </c>
       <c r="B20" s="10">
         <v>1396</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>55</v>
+        <v>184</v>
       </c>
       <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="4" t="s">
-        <v>18</v>
+        <v>132</v>
       </c>
       <c r="B21" s="5">
         <v>1398</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>55</v>
+        <v>184</v>
       </c>
       <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="4" t="s">
-        <v>56</v>
+        <v>185</v>
       </c>
       <c r="B22" s="5">
         <v>1300</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>57</v>
+        <v>186</v>
       </c>
       <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="4" t="s">
-        <v>21</v>
+        <v>135</v>
       </c>
       <c r="B23" s="5">
         <v>1396</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>58</v>
+        <v>187</v>
       </c>
       <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="4" t="s">
-        <v>59</v>
+        <v>188</v>
       </c>
       <c r="B24" s="5">
         <v>1122</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>58</v>
+        <v>187</v>
       </c>
       <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="4" t="s">
-        <v>60</v>
+        <v>189</v>
       </c>
       <c r="B25" s="5">
         <v>1148</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>61</v>
+        <v>190</v>
       </c>
       <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="4" t="s">
-        <v>62</v>
+        <v>191</v>
       </c>
       <c r="B26" s="5">
         <v>915</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>63</v>
+        <v>192</v>
       </c>
       <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="4" t="s">
-        <v>64</v>
+        <v>193</v>
       </c>
       <c r="B27" s="5">
         <v>3523</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>65</v>
+        <v>194</v>
       </c>
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="7" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="B28" s="8">
         <v>207</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>67</v>
+        <v>195</v>
       </c>
       <c r="D28" s="7"/>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="4" t="s">
-        <v>68</v>
+        <v>196</v>
       </c>
       <c r="B29" s="5">
         <v>1389</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>67</v>
+        <v>195</v>
       </c>
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="7" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="B30" s="8">
         <v>151</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>70</v>
+        <v>197</v>
       </c>
       <c r="D30" s="7"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
-        <v>71</v>
+        <v>198</v>
       </c>
       <c r="B31" s="5">
         <v>900</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>70</v>
+        <v>197</v>
       </c>
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
-        <v>72</v>
+        <v>199</v>
       </c>
       <c r="B32" s="5">
         <v>609</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>73</v>
+        <v>200</v>
       </c>
       <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="4" t="s">
-        <v>1</v>
+        <v>115</v>
       </c>
       <c r="B33" s="5">
         <v>1475</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>74</v>
+        <v>201</v>
       </c>
       <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="4" t="s">
-        <v>75</v>
+        <v>202</v>
       </c>
       <c r="B34" s="5">
         <v>633</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>76</v>
+        <v>203</v>
       </c>
       <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="7" t="s">
-        <v>71</v>
+        <v>198</v>
       </c>
       <c r="B35" s="8">
         <v>900</v>
@@ -2096,7 +3549,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:D21"/>
@@ -2117,175 +3570,175 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>77</v>
+        <v>204</v>
       </c>
       <c r="B2" s="5">
         <v>1475</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>78</v>
+        <v>205</v>
       </c>
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>3</v>
+        <v>117</v>
       </c>
       <c r="B3" s="5">
         <v>1470</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>79</v>
+        <v>206</v>
       </c>
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>5</v>
+        <v>119</v>
       </c>
       <c r="B4" s="5">
         <v>1471</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>80</v>
+        <v>207</v>
       </c>
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>81</v>
+        <v>208</v>
       </c>
       <c r="B5" s="5">
         <v>1431</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>80</v>
+        <v>207</v>
       </c>
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>8</v>
+        <v>122</v>
       </c>
       <c r="B6" s="5">
         <v>1408</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>82</v>
+        <v>209</v>
       </c>
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>10</v>
+        <v>124</v>
       </c>
       <c r="B7" s="5">
         <v>1424</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>83</v>
+        <v>210</v>
       </c>
       <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>12</v>
+        <v>126</v>
       </c>
       <c r="B8" s="5">
         <v>1424</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>84</v>
+        <v>211</v>
       </c>
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>16</v>
+        <v>130</v>
       </c>
       <c r="B9" s="5">
         <v>1421</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>85</v>
+        <v>212</v>
       </c>
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>18</v>
+        <v>132</v>
       </c>
       <c r="B10" s="5">
         <v>1398</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>86</v>
+        <v>213</v>
       </c>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="4" t="s">
-        <v>56</v>
+        <v>185</v>
       </c>
       <c r="B11" s="5">
         <v>1300</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>87</v>
+        <v>214</v>
       </c>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="4" t="s">
-        <v>21</v>
+        <v>135</v>
       </c>
       <c r="B12" s="5">
         <v>1396</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>88</v>
+        <v>215</v>
       </c>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="4" t="s">
-        <v>23</v>
+        <v>137</v>
       </c>
       <c r="B13" s="5">
         <v>1424</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>89</v>
+        <v>216</v>
       </c>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="4" t="s">
-        <v>24</v>
+        <v>138</v>
       </c>
       <c r="B14" s="5">
         <v>1398</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>89</v>
+        <v>216</v>
       </c>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="4" t="s">
-        <v>26</v>
+        <v>140</v>
       </c>
       <c r="B15" s="5">
         <v>1396</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>90</v>
+        <v>217</v>
       </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="7" t="s">
-        <v>27</v>
+        <v>141</v>
       </c>
       <c r="B16" s="8">
         <v>1419</v>
@@ -2293,55 +3746,55 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="9" t="s">
-        <v>29</v>
+        <v>143</v>
       </c>
       <c r="B17" s="10">
         <v>1420</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>91</v>
+        <v>218</v>
       </c>
       <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
       <c r="B18" s="5">
         <v>1303</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>92</v>
+        <v>219</v>
       </c>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="4" t="s">
-        <v>93</v>
+        <v>220</v>
       </c>
       <c r="B19" s="5">
         <v>1432</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>94</v>
+        <v>221</v>
       </c>
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
-        <v>34</v>
+        <v>148</v>
       </c>
       <c r="B20" s="5">
         <v>1419</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>94</v>
+        <v>221</v>
       </c>
       <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="7" t="s">
-        <v>77</v>
+        <v>204</v>
       </c>
       <c r="B21" s="8">
         <v>1475</v>
@@ -2353,7 +3806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:A24"/>
@@ -2374,121 +3827,1493 @@
     </row>
     <row r="2" ht="77.25" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" ht="77.25" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>77</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" ht="77.25" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>77</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" ht="77.25" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" ht="90" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>95</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" ht="90" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>95</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" ht="77.25" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" ht="77.25" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" ht="77.25" spans="1:1">
       <c r="A10" s="1" t="s">
-        <v>81</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" ht="77.25" spans="1:1">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" ht="77.25" spans="1:1">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" ht="77.25" spans="1:1">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" ht="64.5" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" ht="77.25" spans="1:1">
       <c r="A15" s="2" t="s">
-        <v>23</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" ht="64.5" spans="1:1">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" ht="77.25" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>10</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" ht="77.25" spans="1:1">
       <c r="A18" s="1" t="s">
-        <v>12</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" ht="77.25" spans="1:1">
       <c r="A19" s="1" t="s">
-        <v>96</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" ht="64.5" spans="1:1">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" ht="64.5" spans="1:1">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" ht="77.25" spans="1:1">
       <c r="A22" s="1" t="s">
-        <v>16</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" ht="77.25" spans="1:1">
       <c r="A23" s="1" t="s">
-        <v>97</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" ht="64.5" spans="1:1">
       <c r="A24" s="3" t="s">
-        <v>21</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="119.428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" ht="15.75" spans="1:7">
+      <c r="A2" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="29">
+        <v>1450</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" spans="1:4">
+      <c r="A3" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="32">
+        <v>1449</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" ht="15.75" spans="1:4">
+      <c r="A4" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="32">
+        <v>1</v>
+      </c>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" ht="15.75" spans="1:4">
+      <c r="A5" s="31"/>
+      <c r="B5" s="32">
+        <v>1450</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="16"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="16"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="22"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="25"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="16"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="16"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="16"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A15:A17">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="119.428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" ht="15.75" spans="1:7">
+      <c r="A2" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="29">
+        <v>1451</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" spans="1:4">
+      <c r="A3" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="32">
+        <v>1450</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" ht="15.75" spans="1:4">
+      <c r="A4" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="35">
+        <v>1449</v>
+      </c>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" ht="15.75" spans="1:4">
+      <c r="A5" s="31"/>
+      <c r="B5" s="32">
+        <v>1450</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="16"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="16"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="22"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="25"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="16"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="16"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="16"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A15:A17">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="119.428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" ht="15.75" spans="1:7">
+      <c r="A2" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="29">
+        <v>1467</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" spans="1:4">
+      <c r="A3" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="32">
+        <v>1451</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" ht="15.75" spans="1:4">
+      <c r="A4" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="32">
+        <v>1449</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" ht="15.75" spans="1:4">
+      <c r="A5" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="32">
+        <v>1450</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="16"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="16"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="22"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="25"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="16"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="16"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="16"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A15:A17">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="119.428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="20">
+        <v>1491</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="23">
+        <v>1486</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="23">
+        <v>1487</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="23">
+        <v>1450</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="23">
+        <v>1428</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="23">
+        <v>1453</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="23">
+        <v>1441</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="23">
+        <v>1440</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="23">
+        <v>1440</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="23">
+        <v>1439</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="23">
+        <v>1435</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="16"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="22"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="25"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="16"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="16"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="16"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A15:A17">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="119.428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="14">
+        <v>188</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="G2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="17">
+        <v>1486</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="17">
+        <v>1487</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="17">
+        <v>1491</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="17">
+        <v>1441</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="17">
+        <v>1440</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="17">
+        <v>1440</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="17">
+        <v>1439</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="17">
+        <v>1435</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="17">
+        <v>1450</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="17">
+        <v>1428</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="16"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="17">
+        <v>1453</v>
+      </c>
+      <c r="D13" s="25"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="16"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="16"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="16"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A15:A17">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="119.428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="17">
+        <v>1428</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="16"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="17">
+        <v>1453</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="17">
+        <v>1441</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="17">
+        <v>1440</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="17">
+        <v>1440</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="17">
+        <v>1439</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="17">
+        <v>1435</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="17">
+        <v>1450</v>
+      </c>
+      <c r="C9" s="18">
+        <v>1</v>
+      </c>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="16"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="16"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="25"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="25"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="16"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="16"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="16"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A15:A17">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="119.428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="16"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="16"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="16"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="16"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="25"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="25"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="16"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="16"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="16"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A19:A21">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="119.428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="14">
+        <v>1491</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="17">
+        <v>1486</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="17">
+        <v>1487</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="17">
+        <v>1428</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="17">
+        <v>1452</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="17">
+        <v>1441</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="17">
+        <v>1440</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="17">
+        <v>1440</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="17">
+        <v>1439</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="17">
+        <v>1435</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="16"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="17">
+        <v>1450</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="16"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="16"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="16"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="25"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="25"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="16"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="16"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="16"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A19:A21">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>